<commit_message>
new file:   practice1/practical1_report.xlsx 	modified:   practice1/practical1_td.xlsx
</commit_message>
<xml_diff>
--- a/practice1/practical1_td.xlsx
+++ b/practice1/practical1_td.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\M2\RIM2DSC\TP\practice1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{642B673F-1D07-4DDD-93B0-D6006148FE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DF9CA7-780F-461E-9D5E-5CDB44C3F422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AB027B67-69EB-4C9A-A926-2B1FB51BD12C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">docID : </t>
   </si>
@@ -45,78 +45,6 @@
   </si>
   <si>
     <t>Term :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please </t>
-  </si>
-  <si>
-    <t>Please</t>
-  </si>
-  <si>
-    <t>Me</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Day </t>
-  </si>
-  <si>
-    <t xml:space="preserve">in </t>
-  </si>
-  <si>
-    <t xml:space="preserve">the </t>
-  </si>
-  <si>
-    <t>Life</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hard </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Day’s </t>
-  </si>
-  <si>
-    <t>Night</t>
-  </si>
-  <si>
-    <t>Long</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Long </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The </t>
-  </si>
-  <si>
-    <t xml:space="preserve">and </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Winding </t>
-  </si>
-  <si>
-    <t>Road</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Love </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Me </t>
-  </si>
-  <si>
-    <t>Do</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You </t>
-  </si>
-  <si>
-    <t>To</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mr </t>
-  </si>
-  <si>
-    <t>Postman</t>
   </si>
 </sst>
 </file>
@@ -132,12 +60,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -154,9 +88,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{343EB5B4-ED26-4434-A187-2E533D4FDDF0}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,160 +414,15 @@
     <col min="4" max="4" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -644,11 +431,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="0e11f74a-6172-4b18-9170-526343e1ecb3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -879,27 +667,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="0e11f74a-6172-4b18-9170-526343e1ecb3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CBB57D8-0660-4F28-8FF2-51FA81A0B47B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{787CBFF5-7BF7-4F7A-9332-4E173FBA47C4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="07e6d9f0-0857-43aa-9f77-41eb654023f0"/>
-    <ds:schemaRef ds:uri="0e11f74a-6172-4b18-9170-526343e1ecb3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -924,9 +702,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{787CBFF5-7BF7-4F7A-9332-4E173FBA47C4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CBB57D8-0660-4F28-8FF2-51FA81A0B47B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="07e6d9f0-0857-43aa-9f77-41eb654023f0"/>
+    <ds:schemaRef ds:uri="0e11f74a-6172-4b18-9170-526343e1ecb3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>